<commit_message>
add second data controls
</commit_message>
<xml_diff>
--- a/ReamesDataTwo.xlsx
+++ b/ReamesDataTwo.xlsx
@@ -1,13 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbearg/Documents/Projects/ReamesViz/reamesmap/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ReamesDataTwo" r:id="rId3" sheetId="1"/>
+    <sheet name="ReamesDataTwo" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -353,13 +360,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -371,7 +375,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -386,22 +390,329 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,7 +741,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -440,13 +751,12 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="n">
-        <v>36.0913</v>
-      </c>
-      <c r="E2" t="n">
-        <v>28.0882</v>
-      </c>
-      <c r="F2"/>
+      <c r="D2">
+        <v>36.091299999999997</v>
+      </c>
+      <c r="E2">
+        <v>28.088200000000001</v>
+      </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
@@ -457,7 +767,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -467,15 +777,14 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="n">
-        <v>36.0913</v>
-      </c>
-      <c r="E3" t="n">
-        <v>28.0882</v>
-      </c>
-      <c r="F3"/>
-      <c r="G3" t="n">
-        <v>325.0</v>
+      <c r="D3">
+        <v>36.091299999999997</v>
+      </c>
+      <c r="E3">
+        <v>28.088200000000001</v>
+      </c>
+      <c r="G3">
+        <v>325</v>
       </c>
       <c r="H3" t="s">
         <v>13</v>
@@ -484,7 +793,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -494,13 +803,12 @@
       <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="n">
-        <v>36.544</v>
-      </c>
-      <c r="E4" t="n">
+      <c r="D4">
+        <v>36.543999999999997</v>
+      </c>
+      <c r="E4">
         <v>26.355</v>
       </c>
-      <c r="F4"/>
       <c r="G4" t="s">
         <v>12</v>
       </c>
@@ -511,7 +819,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -521,13 +829,12 @@
       <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="n">
-        <v>39.1341</v>
-      </c>
-      <c r="E5" t="n">
-        <v>25.9348</v>
-      </c>
-      <c r="F5"/>
+      <c r="D5">
+        <v>39.134099999999997</v>
+      </c>
+      <c r="E5">
+        <v>25.934799999999999</v>
+      </c>
       <c r="G5" t="s">
         <v>23</v>
       </c>
@@ -538,7 +845,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -548,13 +855,12 @@
       <c r="C6" t="s">
         <v>27</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>39.3367</v>
       </c>
-      <c r="E6" t="n">
-        <v>26.6548</v>
-      </c>
-      <c r="F6"/>
+      <c r="E6">
+        <v>26.654800000000002</v>
+      </c>
       <c r="G6" t="s">
         <v>28</v>
       </c>
@@ -565,7 +871,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -575,13 +881,12 @@
       <c r="C7" t="s">
         <v>32</v>
       </c>
-      <c r="D7" t="n">
-        <v>41.287</v>
-      </c>
-      <c r="E7" t="n">
-        <v>31.426</v>
-      </c>
-      <c r="F7"/>
+      <c r="D7">
+        <v>41.286999999999999</v>
+      </c>
+      <c r="E7">
+        <v>31.425999999999998</v>
+      </c>
       <c r="G7" t="s">
         <v>33</v>
       </c>
@@ -592,7 +897,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -602,13 +907,12 @@
       <c r="C8" t="s">
         <v>38</v>
       </c>
-      <c r="D8" t="n">
-        <v>44.6103</v>
-      </c>
-      <c r="E8" t="n">
-        <v>33.4922</v>
-      </c>
-      <c r="F8"/>
+      <c r="D8">
+        <v>44.610300000000002</v>
+      </c>
+      <c r="E8">
+        <v>33.492199999999997</v>
+      </c>
       <c r="G8" t="s">
         <v>23</v>
       </c>
@@ -619,7 +923,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -629,13 +933,12 @@
       <c r="C9" t="s">
         <v>38</v>
       </c>
-      <c r="D9" t="n">
-        <v>44.6103</v>
-      </c>
-      <c r="E9" t="n">
-        <v>33.4922</v>
-      </c>
-      <c r="F9"/>
+      <c r="D9">
+        <v>44.610300000000002</v>
+      </c>
+      <c r="E9">
+        <v>33.492199999999997</v>
+      </c>
       <c r="G9" t="s">
         <v>42</v>
       </c>
@@ -646,7 +949,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -656,13 +959,12 @@
       <c r="C10" t="s">
         <v>38</v>
       </c>
-      <c r="D10" t="n">
-        <v>44.6103</v>
-      </c>
-      <c r="E10" t="n">
-        <v>33.4922</v>
-      </c>
-      <c r="F10"/>
+      <c r="D10">
+        <v>44.610300000000002</v>
+      </c>
+      <c r="E10">
+        <v>33.492199999999997</v>
+      </c>
       <c r="G10" t="s">
         <v>12</v>
       </c>
@@ -673,7 +975,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -683,13 +985,12 @@
       <c r="C11" t="s">
         <v>47</v>
       </c>
-      <c r="D11" t="n">
-        <v>48.8148</v>
-      </c>
-      <c r="E11" t="n">
-        <v>28.5865</v>
-      </c>
-      <c r="F11"/>
+      <c r="D11">
+        <v>48.814799999999998</v>
+      </c>
+      <c r="E11">
+        <v>28.586500000000001</v>
+      </c>
       <c r="G11" t="s">
         <v>12</v>
       </c>
@@ -700,7 +1001,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -710,13 +1011,12 @@
       <c r="C12" t="s">
         <v>51</v>
       </c>
-      <c r="D12" t="n">
-        <v>38.3997</v>
-      </c>
-      <c r="E12" t="n">
-        <v>21.8313</v>
-      </c>
-      <c r="F12"/>
+      <c r="D12">
+        <v>38.399700000000003</v>
+      </c>
+      <c r="E12">
+        <v>21.831299999999999</v>
+      </c>
       <c r="G12" t="s">
         <v>52</v>
       </c>
@@ -727,7 +1027,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -737,13 +1037,12 @@
       <c r="C13" t="s">
         <v>57</v>
       </c>
-      <c r="D13" t="n">
-        <v>38.2935</v>
-      </c>
-      <c r="E13" t="n">
-        <v>23.1549</v>
-      </c>
-      <c r="F13"/>
+      <c r="D13">
+        <v>38.293500000000002</v>
+      </c>
+      <c r="E13">
+        <v>23.154900000000001</v>
+      </c>
       <c r="G13" t="s">
         <v>58</v>
       </c>
@@ -754,7 +1053,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -764,13 +1063,12 @@
       <c r="C14" t="s">
         <v>57</v>
       </c>
-      <c r="D14" t="n">
-        <v>38.2935</v>
-      </c>
-      <c r="E14" t="n">
-        <v>23.1549</v>
-      </c>
-      <c r="F14"/>
+      <c r="D14">
+        <v>38.293500000000002</v>
+      </c>
+      <c r="E14">
+        <v>23.154900000000001</v>
+      </c>
       <c r="G14" t="s">
         <v>61</v>
       </c>
@@ -781,7 +1079,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -791,13 +1089,12 @@
       <c r="C15" t="s">
         <v>65</v>
       </c>
-      <c r="D15" t="n">
-        <v>38.2564</v>
-      </c>
-      <c r="E15" t="n">
-        <v>22.972</v>
-      </c>
-      <c r="F15"/>
+      <c r="D15">
+        <v>38.256399999999999</v>
+      </c>
+      <c r="E15">
+        <v>22.972000000000001</v>
+      </c>
       <c r="G15" t="s">
         <v>23</v>
       </c>
@@ -808,7 +1105,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -818,13 +1115,12 @@
       <c r="C16" t="s">
         <v>69</v>
       </c>
-      <c r="D16" t="n">
-        <v>38.4956</v>
-      </c>
-      <c r="E16" t="n">
-        <v>22.9641</v>
-      </c>
-      <c r="F16"/>
+      <c r="D16">
+        <v>38.495600000000003</v>
+      </c>
+      <c r="E16">
+        <v>22.964099999999998</v>
+      </c>
       <c r="G16" t="s">
         <v>70</v>
       </c>
@@ -835,7 +1131,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>67</v>
       </c>
@@ -845,13 +1141,12 @@
       <c r="C17" t="s">
         <v>73</v>
       </c>
-      <c r="D17" t="n">
-        <v>38.4987</v>
-      </c>
-      <c r="E17" t="n">
+      <c r="D17">
+        <v>38.498699999999999</v>
+      </c>
+      <c r="E17">
         <v>23.448</v>
       </c>
-      <c r="F17"/>
       <c r="G17" t="s">
         <v>74</v>
       </c>
@@ -862,7 +1157,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>76</v>
       </c>
@@ -872,13 +1167,12 @@
       <c r="C18" t="s">
         <v>78</v>
       </c>
-      <c r="D18" t="n">
-        <v>38.4791</v>
-      </c>
-      <c r="E18" t="n">
+      <c r="D18">
+        <v>38.479100000000003</v>
+      </c>
+      <c r="E18">
         <v>22.497</v>
       </c>
-      <c r="F18"/>
       <c r="G18" t="s">
         <v>79</v>
       </c>
@@ -889,7 +1183,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>67</v>
       </c>
@@ -899,13 +1193,12 @@
       <c r="C19" t="s">
         <v>57</v>
       </c>
-      <c r="D19" t="n">
-        <v>38.2935</v>
-      </c>
-      <c r="E19" t="n">
-        <v>23.1549</v>
-      </c>
-      <c r="F19"/>
+      <c r="D19">
+        <v>38.293500000000002</v>
+      </c>
+      <c r="E19">
+        <v>23.154900000000001</v>
+      </c>
       <c r="G19" t="s">
         <v>58</v>
       </c>
@@ -916,7 +1209,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>67</v>
       </c>
@@ -926,13 +1219,12 @@
       <c r="C20" t="s">
         <v>57</v>
       </c>
-      <c r="D20" t="n">
-        <v>38.2935</v>
-      </c>
-      <c r="E20" t="n">
-        <v>23.1549</v>
-      </c>
-      <c r="F20"/>
+      <c r="D20">
+        <v>38.293500000000002</v>
+      </c>
+      <c r="E20">
+        <v>23.154900000000001</v>
+      </c>
       <c r="G20" t="s">
         <v>58</v>
       </c>
@@ -943,7 +1235,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -953,13 +1245,12 @@
       <c r="C21" t="s">
         <v>57</v>
       </c>
-      <c r="D21" t="n">
-        <v>38.2935</v>
-      </c>
-      <c r="E21" t="n">
-        <v>23.1549</v>
-      </c>
-      <c r="F21"/>
+      <c r="D21">
+        <v>38.293500000000002</v>
+      </c>
+      <c r="E21">
+        <v>23.154900000000001</v>
+      </c>
       <c r="G21" t="s">
         <v>61</v>
       </c>
@@ -970,7 +1261,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>67</v>
       </c>
@@ -980,13 +1271,12 @@
       <c r="C22" t="s">
         <v>57</v>
       </c>
-      <c r="D22" t="n">
-        <v>38.2935</v>
-      </c>
-      <c r="E22" t="n">
-        <v>23.1549</v>
-      </c>
-      <c r="F22"/>
+      <c r="D22">
+        <v>38.293500000000002</v>
+      </c>
+      <c r="E22">
+        <v>23.154900000000001</v>
+      </c>
       <c r="G22" t="s">
         <v>83</v>
       </c>
@@ -997,7 +1287,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>85</v>
       </c>
@@ -1007,13 +1297,12 @@
       <c r="C23" t="s">
         <v>87</v>
       </c>
-      <c r="D23" t="n">
-        <v>38.3191</v>
-      </c>
-      <c r="E23" t="n">
-        <v>23.3178</v>
-      </c>
-      <c r="F23"/>
+      <c r="D23">
+        <v>38.319099999999999</v>
+      </c>
+      <c r="E23">
+        <v>23.317799999999998</v>
+      </c>
       <c r="G23" t="s">
         <v>88</v>
       </c>
@@ -1024,7 +1313,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1034,13 +1323,12 @@
       <c r="C24" t="s">
         <v>91</v>
       </c>
-      <c r="D24" t="n">
-        <v>38.6718</v>
-      </c>
-      <c r="E24" t="n">
-        <v>21.3195</v>
-      </c>
-      <c r="F24"/>
+      <c r="D24">
+        <v>38.671799999999998</v>
+      </c>
+      <c r="E24">
+        <v>21.319500000000001</v>
+      </c>
       <c r="G24" t="s">
         <v>92</v>
       </c>
@@ -1051,7 +1339,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -1061,13 +1349,12 @@
       <c r="C25" t="s">
         <v>96</v>
       </c>
-      <c r="D25" t="n">
-        <v>38.1446</v>
-      </c>
-      <c r="E25" t="n">
-        <v>21.5514</v>
-      </c>
-      <c r="F25"/>
+      <c r="D25">
+        <v>38.144599999999997</v>
+      </c>
+      <c r="E25">
+        <v>21.551400000000001</v>
+      </c>
       <c r="G25" t="s">
         <v>12</v>
       </c>
@@ -1078,7 +1365,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>76</v>
       </c>
@@ -1088,15 +1375,14 @@
       <c r="C26" t="s">
         <v>96</v>
       </c>
-      <c r="D26" t="n">
-        <v>38.1446</v>
-      </c>
-      <c r="E26" t="n">
-        <v>21.5514</v>
-      </c>
-      <c r="F26"/>
-      <c r="G26" t="n">
-        <v>219.0</v>
+      <c r="D26">
+        <v>38.144599999999997</v>
+      </c>
+      <c r="E26">
+        <v>21.551400000000001</v>
+      </c>
+      <c r="G26">
+        <v>219</v>
       </c>
       <c r="H26" t="s">
         <v>97</v>
@@ -1105,7 +1391,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -1115,15 +1401,14 @@
       <c r="C27" t="s">
         <v>101</v>
       </c>
-      <c r="D27" t="n">
-        <v>40.476</v>
-      </c>
-      <c r="E27" t="n">
-        <v>17.228</v>
-      </c>
-      <c r="F27"/>
-      <c r="G27" t="n">
-        <v>267.0</v>
+      <c r="D27">
+        <v>40.475999999999999</v>
+      </c>
+      <c r="E27">
+        <v>17.228000000000002</v>
+      </c>
+      <c r="G27">
+        <v>267</v>
       </c>
       <c r="H27" t="s">
         <v>102</v>
@@ -1132,7 +1417,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1142,13 +1427,12 @@
       <c r="C28" t="s">
         <v>105</v>
       </c>
-      <c r="D28" t="n">
-        <v>37.5828</v>
-      </c>
-      <c r="E28" t="n">
-        <v>12.8251</v>
-      </c>
-      <c r="F28"/>
+      <c r="D28">
+        <v>37.582799999999999</v>
+      </c>
+      <c r="E28">
+        <v>12.825100000000001</v>
+      </c>
       <c r="G28" t="s">
         <v>92</v>
       </c>
@@ -1159,7 +1443,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -1169,13 +1453,12 @@
       <c r="C29" t="s">
         <v>109</v>
       </c>
-      <c r="D29" t="n">
+      <c r="D29">
         <v>31.5</v>
       </c>
-      <c r="E29" t="n">
+      <c r="E29">
         <v>25.5</v>
       </c>
-      <c r="F29"/>
       <c r="G29" t="s">
         <v>12</v>
       </c>
@@ -1187,6 +1470,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>